<commit_message>
Update Template.xlsx binary file
The binary file `Template.xlsx` has been modified. The specific changes within the file are not detailed in the diff output, but the file content has been altered.
</commit_message>
<xml_diff>
--- a/Demo/Template.xlsx
+++ b/Demo/Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erekl\source\repos\DemoProject\Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erekl\source\repos\DemoProject\ReportGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3592A71-9A21-48DB-A20E-A7C65D0FDB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5406B9C6-F05E-4376-8FDE-503DD2D08D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="135" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>